<commit_message>
Feature : adjust sample xlsx file. adjust import-export excel with right attributes name.
</commit_message>
<xml_diff>
--- a/public/import_templates/ErrorMachineTemplate.xlsx
+++ b/public/import_templates/ErrorMachineTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MES\BE_MES_BTDX\public\import_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\project\php\BE_MES_TBDX\public\import_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8718596-E459-46A3-9EE6-F7AC62E991EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FE8A01-9880-46A2-A6C7-FDB4BE7BB2C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9540" yWindow="2085" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3450" yWindow="2700" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>Công đoạn</t>
   </si>
   <si>
@@ -50,6 +47,9 @@
   </si>
   <si>
     <t>cach_xu_ly</t>
+  </si>
+  <si>
+    <t>ten_su_co</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
   <dimension ref="A2:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,33 +453,33 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>